<commit_message>
Got Specs from Desktop
</commit_message>
<xml_diff>
--- a/Algoritmia/Assignment 1/Data Collected.xlsx
+++ b/Algoritmia/Assignment 1/Data Collected.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime Alonso\Documents\UNIOVI\2ndo\Algoritmia\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIOVI\2º\Segundo Semestre\University-2nd\Algoritmia\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F241F4F-3110-4C42-96C0-6BF05FC0C729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8391AD21-D13F-4577-AA8F-C8D25EFCD6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{187FB27A-9F62-409F-87F7-6FA707C05920}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{187FB27A-9F62-409F-87F7-6FA707C05920}"/>
   </bookViews>
   <sheets>
     <sheet name="PythonA1 time measures" sheetId="1" r:id="rId1"/>
-    <sheet name="Laptop Specs" sheetId="2" r:id="rId2"/>
+    <sheet name="Desktop Specs" sheetId="3" r:id="rId2"/>
+    <sheet name="Laptop Specs" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>n</t>
   </si>
@@ -76,6 +77,12 @@
   </si>
   <si>
     <t>NVIDIA GeForce RTX 4050 Laptop GPU</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7 3700X 8-Core Processor 3600Mhz</t>
+  </si>
+  <si>
+    <t>NVIDIA GeForce RTX 3060</t>
   </si>
 </sst>
 </file>
@@ -135,7 +142,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -433,16 +440,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E0A44F-A1BD-4287-936F-2677F3E1FA8D}">
   <dimension ref="B3:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -452,7 +459,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -466,7 +473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1000</v>
       </c>
@@ -476,11 +483,11 @@
       <c r="E5">
         <v>1000</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="1">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2000</v>
       </c>
@@ -490,11 +497,11 @@
       <c r="E6">
         <v>2000</v>
       </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="1">
+        <v>7825</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4000</v>
       </c>
@@ -504,11 +511,11 @@
       <c r="E7">
         <v>4000</v>
       </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F7" s="1">
+        <v>31984</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>8000</v>
       </c>
@@ -522,7 +529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>16000</v>
       </c>
@@ -536,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>32000</v>
       </c>
@@ -550,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>640000</v>
       </c>
@@ -574,20 +581,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EBE8C9-C48D-4A1A-8B78-066095CEA9DA}">
+  <dimension ref="C6:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844379A8-54CB-4931-885E-5028A683806F}">
   <dimension ref="C5:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -595,7 +645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -603,7 +653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Measures taken, document must be done
</commit_message>
<xml_diff>
--- a/Algoritmia/Assignment 1/Data Collected.xlsx
+++ b/Algoritmia/Assignment 1/Data Collected.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIOVI\2º\Segundo Semestre\University-2nd\Algoritmia\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime Alonso\Documents\UNIOVI\2ndo\Algoritmia\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8391AD21-D13F-4577-AA8F-C8D25EFCD6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DDBCF1-E6A8-48CA-A911-9FE075EDCBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{187FB27A-9F62-409F-87F7-6FA707C05920}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{187FB27A-9F62-409F-87F7-6FA707C05920}"/>
   </bookViews>
   <sheets>
-    <sheet name="PythonA1 time measures" sheetId="1" r:id="rId1"/>
-    <sheet name="Desktop Specs" sheetId="3" r:id="rId2"/>
-    <sheet name="Laptop Specs" sheetId="2" r:id="rId3"/>
+    <sheet name="A1 time measures" sheetId="1" r:id="rId1"/>
+    <sheet name="A2 time measures" sheetId="4" r:id="rId2"/>
+    <sheet name="A3 time measures" sheetId="5" r:id="rId3"/>
+    <sheet name="Desktop Specs" sheetId="3" r:id="rId4"/>
+    <sheet name="Laptop Specs" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>n</t>
   </si>
@@ -83,6 +85,180 @@
   </si>
   <si>
     <t>NVIDIA GeForce RTX 3060</t>
+  </si>
+  <si>
+    <t>PYTHON</t>
+  </si>
+  <si>
+    <t>JAVA</t>
+  </si>
+  <si>
+    <t>OPTIMIZED</t>
+  </si>
+  <si>
+    <t>NOT OPTIMIZED</t>
+  </si>
+  <si>
+    <t>1,956</t>
+  </si>
+  <si>
+    <t>7,825</t>
+  </si>
+  <si>
+    <t>31,984</t>
+  </si>
+  <si>
+    <t>0,047</t>
+  </si>
+  <si>
+    <t>0,081</t>
+  </si>
+  <si>
+    <t>0,321</t>
+  </si>
+  <si>
+    <t>1,271</t>
+  </si>
+  <si>
+    <t>5,201</t>
+  </si>
+  <si>
+    <t>20,321</t>
+  </si>
+  <si>
+    <t>80,967 (OoT)</t>
+  </si>
+  <si>
+    <t>0,368</t>
+  </si>
+  <si>
+    <t>1,604</t>
+  </si>
+  <si>
+    <t>6,453</t>
+  </si>
+  <si>
+    <t>25,509</t>
+  </si>
+  <si>
+    <t>108,213(OoT)</t>
+  </si>
+  <si>
+    <t>0,011</t>
+  </si>
+  <si>
+    <t>0,035</t>
+  </si>
+  <si>
+    <t>0,1274</t>
+  </si>
+  <si>
+    <t>0,478</t>
+  </si>
+  <si>
+    <t>1,841</t>
+  </si>
+  <si>
+    <t>6,835</t>
+  </si>
+  <si>
+    <t>25,898</t>
+  </si>
+  <si>
+    <t>0,173</t>
+  </si>
+  <si>
+    <t>0,634</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>9,076</t>
+  </si>
+  <si>
+    <t>34,817</t>
+  </si>
+  <si>
+    <t>130,778(OoT)</t>
+  </si>
+  <si>
+    <t>0,008</t>
+  </si>
+  <si>
+    <t>0,017</t>
+  </si>
+  <si>
+    <t>0,272</t>
+  </si>
+  <si>
+    <t>0,990</t>
+  </si>
+  <si>
+    <t>3,757</t>
+  </si>
+  <si>
+    <t>13,989</t>
+  </si>
+  <si>
+    <t>0,066</t>
+  </si>
+  <si>
+    <t>0,236</t>
+  </si>
+  <si>
+    <t>0,895</t>
+  </si>
+  <si>
+    <t>3,411</t>
+  </si>
+  <si>
+    <t>13,206</t>
+  </si>
+  <si>
+    <t>0,074</t>
+  </si>
+  <si>
+    <t>52,843</t>
+  </si>
+  <si>
+    <t>196,632(OoT)</t>
+  </si>
+  <si>
+    <t>0,208</t>
+  </si>
+  <si>
+    <t>0,796</t>
+  </si>
+  <si>
+    <t>3,015</t>
+  </si>
+  <si>
+    <t>159,755(OoT)</t>
+  </si>
+  <si>
+    <t>0,113</t>
+  </si>
+  <si>
+    <t>0,396</t>
+  </si>
+  <si>
+    <t>1,567</t>
+  </si>
+  <si>
+    <t>6,004</t>
+  </si>
+  <si>
+    <t>56,543</t>
+  </si>
+  <si>
+    <t>215,087 (OoT)</t>
+  </si>
+  <si>
+    <t>23,837</t>
+  </si>
+  <si>
+    <t>113,556(OoT)</t>
   </si>
 </sst>
 </file>
@@ -142,7 +318,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -438,18 +614,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E0A44F-A1BD-4287-936F-2677F3E1FA8D}">
-  <dimension ref="B3:F11"/>
+  <dimension ref="B2:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -458,8 +652,16 @@
         <v>7</v>
       </c>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -472,92 +674,176 @@
       <c r="F4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E5">
-        <v>1000</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1956</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>10000</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <v>10000</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="E6">
-        <v>2000</v>
-      </c>
-      <c r="F6" s="1">
-        <v>7825</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>20000</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>20000</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6">
+        <v>20000</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7">
-        <v>4000</v>
+        <v>40000</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>4000</v>
-      </c>
-      <c r="F7" s="1">
-        <v>31984</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>40000</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>40000</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>40000</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8">
-        <v>8000</v>
+        <v>80000</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="E8">
-        <v>8000</v>
+        <v>80000</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>80000</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8">
+        <v>80000</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9">
-        <v>16000</v>
+        <v>160000</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="E9">
-        <v>16000</v>
+        <v>160000</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>160000</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9">
+        <v>160000</v>
+      </c>
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10">
-        <v>32000</v>
+        <v>320000</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="E10">
-        <v>32000</v>
+        <v>320000</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>320000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10">
+        <v>320000</v>
+      </c>
+      <c r="L10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>640000</v>
       </c>
@@ -570,17 +856,535 @@
       <c r="F11" t="s">
         <v>5</v>
       </c>
+      <c r="H11">
+        <v>640000</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>640000</v>
+      </c>
+      <c r="L11" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F218FBE7-D8F5-4B30-BC20-81DA104BA9A2}">
+  <dimension ref="B3:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6">
+        <v>10000</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="H6">
+        <v>10000</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6">
+        <v>10000</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>20000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7">
+        <v>20000</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="H7">
+        <v>20000</v>
+      </c>
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7">
+        <v>20000</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>40000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8">
+        <v>40000</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="H8">
+        <v>40000</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8">
+        <v>40000</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>80000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9">
+        <v>80000</v>
+      </c>
+      <c r="H9">
+        <v>80000</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9">
+        <v>80000</v>
+      </c>
+      <c r="L9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>160000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10">
+        <v>160000</v>
+      </c>
+      <c r="H10">
+        <v>160000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10">
+        <v>160000</v>
+      </c>
+      <c r="L10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>320000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11">
+        <v>320000</v>
+      </c>
+      <c r="H11">
+        <v>320000</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11">
+        <v>320000</v>
+      </c>
+      <c r="L11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>640000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>640000</v>
+      </c>
+      <c r="H12">
+        <v>640000</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12">
+        <v>640000</v>
+      </c>
+      <c r="L12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K4:L4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EF9B21-503D-446D-9827-6963B381E138}">
+  <dimension ref="B3:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6">
+        <v>10000</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="H6">
+        <v>10000</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6">
+        <v>10000</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>20000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7">
+        <v>20000</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="H7">
+        <v>20000</v>
+      </c>
+      <c r="I7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7">
+        <v>20000</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>40000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8">
+        <v>40000</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="H8">
+        <v>40000</v>
+      </c>
+      <c r="I8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8">
+        <v>40000</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>80000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9">
+        <v>80000</v>
+      </c>
+      <c r="H9">
+        <v>80000</v>
+      </c>
+      <c r="I9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9">
+        <v>80000</v>
+      </c>
+      <c r="L9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>160000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10">
+        <v>160000</v>
+      </c>
+      <c r="H10">
+        <v>160000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10">
+        <v>160000</v>
+      </c>
+      <c r="L10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>320000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11">
+        <v>320000</v>
+      </c>
+      <c r="H11">
+        <v>320000</v>
+      </c>
+      <c r="I11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11">
+        <v>320000</v>
+      </c>
+      <c r="L11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>640000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>640000</v>
+      </c>
+      <c r="H12">
+        <v>640000</v>
+      </c>
+      <c r="I12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12">
+        <v>640000</v>
+      </c>
+      <c r="L12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K4:L4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EBE8C9-C48D-4A1A-8B78-066095CEA9DA}">
   <dimension ref="C6:D8"/>
   <sheetViews>
@@ -588,13 +1392,13 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -602,7 +1406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -610,7 +1414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -623,7 +1427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844379A8-54CB-4931-885E-5028A683806F}">
   <dimension ref="C5:D7"/>
   <sheetViews>
@@ -631,13 +1435,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -645,7 +1449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -653,7 +1457,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Assignment 1 missing conclusion (algorithmics)
</commit_message>
<xml_diff>
--- a/Algoritmia/Assignment 1/Data Collected.xlsx
+++ b/Algoritmia/Assignment 1/Data Collected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime Alonso\Documents\UNIOVI\2ndo\Algoritmia\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DDBCF1-E6A8-48CA-A911-9FE075EDCBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C6085C-E9FF-450A-8F62-BFED48FD9A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{187FB27A-9F62-409F-87F7-6FA707C05920}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="2" activeTab="2" xr2:uid="{187FB27A-9F62-409F-87F7-6FA707C05920}"/>
   </bookViews>
   <sheets>
     <sheet name="A1 time measures" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t>n</t>
   </si>
@@ -48,15 +48,6 @@
     <t>Time(s)</t>
   </si>
   <si>
-    <t>1,763</t>
-  </si>
-  <si>
-    <t>7,6</t>
-  </si>
-  <si>
-    <t>30,206</t>
-  </si>
-  <si>
     <t>OoT</t>
   </si>
   <si>
@@ -109,24 +100,6 @@
   </si>
   <si>
     <t>0,047</t>
-  </si>
-  <si>
-    <t>0,081</t>
-  </si>
-  <si>
-    <t>0,321</t>
-  </si>
-  <si>
-    <t>1,271</t>
-  </si>
-  <si>
-    <t>5,201</t>
-  </si>
-  <si>
-    <t>20,321</t>
-  </si>
-  <si>
-    <t>80,967 (OoT)</t>
   </si>
   <si>
     <t>0,368</t>
@@ -265,10 +238,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -294,12 +276,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -315,6 +299,1127 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>PythonA1.py</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'A1 time measures'!$B$5:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'A1 time measures'!$C$5:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.7629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.206</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119.181</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-89AC-463C-893B-6BEB6F2672D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>JavaA1.java</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'A1 time measures'!$H$5:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'A1 time measures'!$I$5:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.1000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2709999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2009999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.321000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.966999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-89AC-463C-893B-6BEB6F2672D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="131410655"/>
+        <c:axId val="1282181519"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="131410655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="400000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Value (n)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1282181519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1282181519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="131410655"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05805C40-5CE2-D291-22D9-F34C60A60DAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -614,14 +1719,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E0A44F-A1BD-4287-936F-2677F3E1FA8D}">
-  <dimension ref="B2:L11"/>
+  <dimension ref="B2:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
@@ -629,14 +1735,14 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -645,19 +1751,19 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -691,183 +1797,176 @@
       <c r="B5">
         <v>10000</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
+      <c r="C5" s="3">
+        <v>1.7629999999999999</v>
       </c>
       <c r="E5">
         <v>10000</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H5">
         <v>10000</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>23</v>
+      <c r="I5" s="4">
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="K5">
         <v>10000</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>20000</v>
       </c>
-      <c r="C6" t="s">
-        <v>3</v>
+      <c r="C6" s="3">
+        <v>7.6</v>
       </c>
       <c r="E6">
         <v>20000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H6">
         <v>20000</v>
       </c>
-      <c r="I6" t="s">
-        <v>24</v>
+      <c r="I6" s="4">
+        <v>0.32100000000000001</v>
       </c>
       <c r="K6">
         <v>20000</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>40000</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
+      <c r="C7" s="3">
+        <v>30.206</v>
       </c>
       <c r="E7">
         <v>40000</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H7">
         <v>40000</v>
       </c>
-      <c r="I7" t="s">
-        <v>25</v>
+      <c r="I7" s="4">
+        <v>1.2709999999999999</v>
       </c>
       <c r="K7">
         <v>40000</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>80000</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
+      <c r="C8" s="3">
+        <v>119.181</v>
       </c>
       <c r="E8">
         <v>80000</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <v>80000</v>
       </c>
-      <c r="I8" t="s">
-        <v>26</v>
+      <c r="I8" s="4">
+        <v>5.2009999999999996</v>
       </c>
       <c r="K8">
         <v>80000</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>160000</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="E9">
         <v>160000</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>160000</v>
       </c>
-      <c r="I9" t="s">
-        <v>27</v>
+      <c r="I9" s="4">
+        <v>20.321000000000002</v>
       </c>
       <c r="K9">
         <v>160000</v>
       </c>
       <c r="L9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>320000</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
       <c r="E10">
         <v>320000</v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <v>320000</v>
       </c>
-      <c r="I10" t="s">
-        <v>28</v>
+      <c r="I10" s="4">
+        <v>80.966999999999999</v>
       </c>
       <c r="K10">
         <v>320000</v>
       </c>
       <c r="L10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>640000</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
       <c r="E11">
         <v>640000</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <v>640000</v>
       </c>
-      <c r="I11" t="s">
-        <v>5</v>
-      </c>
+      <c r="I11" s="4"/>
       <c r="K11">
         <v>640000</v>
       </c>
       <c r="L11" t="s">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -878,7 +1977,9 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="K3:L3"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -886,7 +1987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F218FBE7-D8F5-4B30-BC20-81DA104BA9A2}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -898,14 +1999,14 @@
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -914,19 +2015,19 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I4" s="2"/>
       <c r="K4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -961,7 +2062,7 @@
         <v>10000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E6">
         <v>10000</v>
@@ -971,13 +2072,13 @@
         <v>10000</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="K6">
         <v>10000</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
@@ -985,7 +2086,7 @@
         <v>20000</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E7">
         <v>20000</v>
@@ -995,13 +2096,13 @@
         <v>20000</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="K7">
         <v>20000</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -1009,7 +2110,7 @@
         <v>40000</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E8">
         <v>40000</v>
@@ -1019,13 +2120,13 @@
         <v>40000</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="K8">
         <v>40000</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
@@ -1033,7 +2134,7 @@
         <v>80000</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E9">
         <v>80000</v>
@@ -1042,13 +2143,13 @@
         <v>80000</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="K9">
         <v>80000</v>
       </c>
       <c r="L9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -1056,7 +2157,7 @@
         <v>160000</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E10">
         <v>160000</v>
@@ -1065,13 +2166,13 @@
         <v>160000</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="K10">
         <v>160000</v>
       </c>
       <c r="L10" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
@@ -1079,7 +2180,7 @@
         <v>320000</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E11">
         <v>320000</v>
@@ -1088,13 +2189,13 @@
         <v>320000</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="K11">
         <v>320000</v>
       </c>
       <c r="L11" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
@@ -1102,7 +2203,7 @@
         <v>640000</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>640000</v>
@@ -1111,13 +2212,13 @@
         <v>640000</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="K12">
         <v>640000</v>
       </c>
       <c r="L12" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1137,7 +2238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EF9B21-503D-446D-9827-6963B381E138}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1149,14 +2250,14 @@
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1165,19 +2266,19 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I4" s="2"/>
       <c r="K4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -1212,7 +2313,7 @@
         <v>10000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E6">
         <v>10000</v>
@@ -1222,13 +2323,13 @@
         <v>10000</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="K6">
         <v>10000</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
@@ -1236,7 +2337,7 @@
         <v>20000</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E7">
         <v>20000</v>
@@ -1246,13 +2347,13 @@
         <v>20000</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="K7">
         <v>20000</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -1260,7 +2361,7 @@
         <v>40000</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E8">
         <v>40000</v>
@@ -1270,13 +2371,13 @@
         <v>40000</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="K8">
         <v>40000</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
@@ -1284,7 +2385,7 @@
         <v>80000</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E9">
         <v>80000</v>
@@ -1293,13 +2394,13 @@
         <v>80000</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="K9">
         <v>80000</v>
       </c>
       <c r="L9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -1307,7 +2408,7 @@
         <v>160000</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E10">
         <v>160000</v>
@@ -1316,13 +2417,13 @@
         <v>160000</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="K10">
         <v>160000</v>
       </c>
       <c r="L10" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
@@ -1330,7 +2431,7 @@
         <v>320000</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E11">
         <v>320000</v>
@@ -1339,13 +2440,13 @@
         <v>320000</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K11">
         <v>320000</v>
       </c>
       <c r="L11" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
@@ -1353,7 +2454,7 @@
         <v>640000</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>640000</v>
@@ -1362,13 +2463,13 @@
         <v>640000</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K12">
         <v>640000</v>
       </c>
       <c r="L12" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1400,15 +2501,15 @@
   <sheetData>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>16</v>
@@ -1416,10 +2517,10 @@
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1443,15 +2544,15 @@
   <sheetData>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>16</v>
@@ -1459,10 +2560,10 @@
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>